<commit_message>
Update cong tac vien
</commit_message>
<xml_diff>
--- a/Todo - List Dragon Gold.xlsx
+++ b/Todo - List Dragon Gold.xlsx
@@ -8,27 +8,30 @@
   </bookViews>
   <sheets>
     <sheet name="Sep" sheetId="5" r:id="rId1"/>
-    <sheet name="Ngan - HCNS" sheetId="1" r:id="rId2"/>
-    <sheet name="Vu - TDCS" sheetId="3" r:id="rId3"/>
-    <sheet name="Tuan - web" sheetId="6" r:id="rId4"/>
+    <sheet name="Hoi dong nghiep" sheetId="1" r:id="rId2"/>
+    <sheet name="Tuan - web" sheetId="6" r:id="rId3"/>
+    <sheet name="Tim hoc vien" sheetId="16" r:id="rId4"/>
     <sheet name="Website" sheetId="10" r:id="rId5"/>
-    <sheet name="Tim hoc vien" sheetId="16" r:id="rId6"/>
-    <sheet name="Marketing" sheetId="14" r:id="rId7"/>
-    <sheet name="Day hoc" sheetId="15" r:id="rId8"/>
-    <sheet name="Học thêm" sheetId="17" r:id="rId9"/>
+    <sheet name="Marketing" sheetId="14" r:id="rId6"/>
+    <sheet name="Day hoc" sheetId="15" r:id="rId7"/>
+    <sheet name="Học thêm" sheetId="17" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Học thêm'!$A$1:$C$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sep!$A$2:$F$18</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tuan - web'!$A$2:$C$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Website!$A$1:$F$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Day hoc'!$A$1:$G$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Học thêm'!$A$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Hoi dong nghiep'!$A$2:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Marketing!$A$1:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sep!$A$2:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tim hoc vien'!$A$1:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tuan - web'!$A$2:$C$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Website!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
   <si>
     <t>STT</t>
   </si>
@@ -42,9 +45,6 @@
     <t>Câu hỏi gửi Tuấn - công ty web Toàn Năng</t>
   </si>
   <si>
-    <t>Công việc gửi Vụ - Phòng tuyển dụng chiêu sinh</t>
-  </si>
-  <si>
     <t>Công việc gửi Ngân - Phòng HCNS</t>
   </si>
   <si>
@@ -114,9 +114,6 @@
     <t>Kiểu công việc</t>
   </si>
   <si>
-    <t>Kiểm tra xem Tuấn nhắc kỹ thuật đã làm hết chưa? Deadline là 21/9/2018</t>
-  </si>
-  <si>
     <t>Đưa mã gtag.js vào trang web</t>
   </si>
   <si>
@@ -168,18 +165,12 @@
     <t>Không khẩn cấp - Quan trọng</t>
   </si>
   <si>
-    <t>0. Tìm đầu vào</t>
-  </si>
-  <si>
     <t>Giá của sản phẩm (vd Macbook) nên để là 23.000.000 chứ không phải 23.000k</t>
   </si>
   <si>
     <t>Không Khẩn cấp - Quan trọng</t>
   </si>
   <si>
-    <t>Thêm thông tin Liên hệ với doanh nghiệp trong mục giới thiệu: thêm page liên hệ làm liên kết nội bộ</t>
-  </si>
-  <si>
     <t>Chưa làm</t>
   </si>
   <si>
@@ -189,15 +180,6 @@
     <t>Menu Sản phẩm hàng hoá khi bấm vào trên tab vẫn còn chữ LƯU TRỮ.</t>
   </si>
   <si>
-    <t>Mỗi buổi 1 tin: 3 tin/ ngày</t>
-  </si>
-  <si>
-    <t>Thêm cái bài post vào mục lĩnh vực hoạt động trên homepage cho đủ 24 lĩnh vực hoạt động</t>
-  </si>
-  <si>
-    <t>Phân loại mục Tuyển Dụng thành các chuyên mục con cho phù hợp với 15 nhóm ngành nghề của công ty</t>
-  </si>
-  <si>
     <t>Làm vào buổi sáng</t>
   </si>
   <si>
@@ -234,70 +216,16 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Tạo bài viết mới trên website cảm nhận học viên bằng video</t>
-  </si>
-  <si>
-    <t>Thêm kênh Youtube vào footer trang web</t>
-  </si>
-  <si>
     <t>Lập Account Twitter, Instagram, LinkedIn, Pinterest, G+</t>
   </si>
   <si>
     <t>Mô tả của 2 mục ở homepage tuyển dụng doanh nghiệp, chiêu sinh đào tạo bị hư</t>
   </si>
   <si>
-    <t>Đọc sách Ebook mà thầy tặng kèm về SEO</t>
-  </si>
-  <si>
-    <t>Kiến nghị làm kênh Youtube upload và cho đăng các bài giảng</t>
-  </si>
-  <si>
-    <t>Chưa xong</t>
-  </si>
-  <si>
     <t>Thêm content cho thẻ meta description trên homepage như thế nào</t>
   </si>
   <si>
-    <t>Tải ảnh lên Drive: hội thảo với sv đại học cần thơ khoa công nghệ</t>
-  </si>
-  <si>
-    <t>Chọn ra những tấm đẹp nhất</t>
-  </si>
-  <si>
-    <t>Chỉnh sáng tối các tấm ảnh</t>
-  </si>
-  <si>
-    <t>Up lên Slider</t>
-  </si>
-  <si>
-    <t>Thêm Video sáng nay vào mục hoạt động công ty trong menu tin tức</t>
-  </si>
-  <si>
-    <t>Thêm 2 video cảm nghĩ học viên vào mục hoạt động công ty</t>
-  </si>
-  <si>
     <t>Cty bên quản trị mạng sử dụng hệ điều hành gì</t>
-  </si>
-  <si>
-    <t>Tải ảnh xuống máy tính từ Drive hội thảo với sv đại học Cần Thơ khoa công nghệ</t>
-  </si>
-  <si>
-    <t>Tải video lên youtube</t>
-  </si>
-  <si>
-    <t>Thêm menu tin "hoạt động công ty" vào mục tin tức</t>
-  </si>
-  <si>
-    <t>Sửa lại Homepage chữ Lĩnh vực hoạt động thành Hoạt động Công ty rồi đưa những bài có liên quan lên</t>
-  </si>
-  <si>
-    <t>Thời gian có thể đưa bạn Thành qua bên cty kia để làm</t>
-  </si>
-  <si>
-    <t>Đồng nghiệp</t>
-  </si>
-  <si>
-    <t>Thêm logo các trường đại học</t>
   </si>
   <si>
     <t>Mũi tên trên slider của website mobile bỏ đi</t>
@@ -328,6 +256,48 @@
   </si>
   <si>
     <t>Đăng tin trên các trang đăng tuyển việc làm</t>
+  </si>
+  <si>
+    <t>Gửi thông tin tuyển dụng cho Danh Giận trên Messenger</t>
+  </si>
+  <si>
+    <t>Tên Đồng Nghiệp</t>
+  </si>
+  <si>
+    <t>Phòng</t>
+  </si>
+  <si>
+    <t>Loại công việc</t>
+  </si>
+  <si>
+    <t>Ngân</t>
+  </si>
+  <si>
+    <t>Vụ</t>
+  </si>
+  <si>
+    <t>TD-CS</t>
+  </si>
+  <si>
+    <t>HCNS</t>
+  </si>
+  <si>
+    <t>Đưa nội dung tài liệu về dạy học lên gg drive</t>
+  </si>
+  <si>
+    <t>Nêu những câu hỏi của cac ban sv trong video dài</t>
+  </si>
+  <si>
+    <t>Đăng tin lên các group được thông báo trong notification</t>
+  </si>
+  <si>
+    <t>Học bài SEO trong folder SEO</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem Tuấn nhắc kỹ thuật đã làm hết chưa</t>
+  </si>
+  <si>
+    <t>Nêu nội dung clip trong video ngắn</t>
   </si>
 </sst>
 </file>
@@ -413,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -523,9 +493,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -838,11 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +822,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,265 +833,258 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(B3="", "", SUBTOTAL(3,$B3:B$3))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(B4="", "", SUBTOTAL(3,$B$3:B4))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="34"/>
     </row>
-    <row r="5" spans="1:6" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(B5="", "", SUBTOTAL(3,$B$3:B5))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="34"/>
     </row>
-    <row r="6" spans="1:6" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(B6="", "", SUBTOTAL(3,$B$3:B6))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="34"/>
     </row>
-    <row r="7" spans="1:6" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f>IF(B7="", "", SUBTOTAL(3,$B$3:B7))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:6" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f>IF(B8="", "", SUBTOTAL(3,$B$3:B8))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f>IF(B9="", "", SUBTOTAL(3,$B$3:B9))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>8</v>
-      </c>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>IF(B10="", "", SUBTOTAL(3,$B$3:B10))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f>IF(B11="", "", SUBTOTAL(3,$B$3:B11))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:6" ht="43.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f>IF(B12="", "", SUBTOTAL(3,$B$3:B12))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <f>IF(B13="", "", SUBTOTAL(3,$B$3:B13))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f>IF(B14="", "", SUBTOTAL(3,$B$3:B14))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <f>IF(B15="", "", SUBTOTAL(3,$B$3:B15))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <f>IF(B16="", "", SUBTOTAL(3,$B$3:B16))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="7" t="str">
         <f>IF(B17="", "", SUBTOTAL(3,$B$3:B17))</f>
-        <v>1</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>73</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B17" s="12"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="11" t="s">
-        <v>74</v>
-      </c>
+      <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="str">
-        <f>IF(B18="", "", SUBTOTAL(3,$B$3:B18))</f>
-        <v/>
-      </c>
+    <row r="18" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" s="12"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -1159,7 +1118,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="11"/>
@@ -1174,18 +1133,15 @@
       <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="17"/>
     </row>
     <row r="28" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1196,8 +1152,7 @@
       <c r="B29" s="17"/>
     </row>
     <row r="30" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="14"/>
     </row>
     <row r="31" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
@@ -1223,7 +1178,7 @@
     <row r="38" spans="2:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
     </row>
-    <row r="39" spans="2:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
@@ -1241,17 +1196,8 @@
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:F18">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Chưa xong"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:F17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1259,24 +1205,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1284,56 +1237,83 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1364,133 +1344,13 @@
     <row r="32" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="A2:G4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D27"/>
@@ -1520,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,10 +1389,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,10 +1401,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1553,10 +1413,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,10 +1425,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1577,10 +1437,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,10 +1449,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,10 +1473,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,10 +1485,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1661,10 +1521,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1697,10 +1557,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -1777,19 +1637,211 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <f>IF(B2="","",SUBTOTAL(3,$B$2:B2))</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <f>IF(B3="","",SUBTOTAL(3,$B$2:B3))</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <f>IF(B4="","",SUBTOTAL(3,$B$2:B4))</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <f>IF(B5="","",SUBTOTAL(3,$B$2:B5))</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <f>IF(B6="","",SUBTOTAL(3,$B$2:B6))</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <f>IF(B7="","",SUBTOTAL(3,$B$2:B7))</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <f>IF(B8="","",SUBTOTAL(3,$B$2:B8))</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="str">
+        <f>IF(B9="","",SUBTOTAL(3,$B$2:B9))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="str">
+        <f>IF(B10="","",SUBTOTAL(3,$B$2:B10))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <autoFilter ref="A1:D10"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47" style="14" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
@@ -1807,70 +1859,70 @@
         <v>2</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <f>IF(B2="","",SUBTOTAL(3,$B$2:B2))</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="39">
-        <v>1</v>
-      </c>
-      <c r="E2" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="38">
+        <v>1</v>
+      </c>
+      <c r="E2" s="35"/>
       <c r="F2" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <f>IF(B3="","",SUBTOTAL(3,$B$2:B3))</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="39">
-        <v>1</v>
-      </c>
-      <c r="E3" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="38">
+        <v>1</v>
+      </c>
+      <c r="E3" s="35"/>
       <c r="F3" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <f>IF(B4="","",SUBTOTAL(3,$B$2:B4))</f>
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="39">
-        <v>1</v>
-      </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35" t="s">
-        <v>48</v>
+      <c r="B4" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1878,290 +1930,138 @@
         <f>IF(B5="","",SUBTOTAL(3,$B$2:B5))</f>
         <v>2</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="39">
-        <v>1</v>
-      </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <f>IF(B6="","",SUBTOTAL(3,$B$2:B6))</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="37" t="s">
-        <v>56</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="str">
         <f>IF(B7="","",SUBTOTAL(3,$B$2:B7))</f>
-        <v>2</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+        <v/>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="str">
         <f>IF(B8="","",SUBTOTAL(3,$B$2:B8))</f>
-        <v>3</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+        <v/>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="str">
         <f>IF(B9="","",SUBTOTAL(3,$B$2:B9))</f>
-        <v>4</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26">
+        <v/>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="str">
         <f>IF(B10="","",SUBTOTAL(3,$B$2:B10))</f>
-        <v>4</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
+        <v/>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="str">
         <f>IF(B11="","",SUBTOTAL(3,$B$2:B11))</f>
-        <v>4</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26">
+        <v/>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="str">
         <f>IF(B12="","",SUBTOTAL(3,$B$2:B12))</f>
-        <v>5</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="str">
         <f>IF(B13="","",SUBTOTAL(3,$B$2:B13))</f>
-        <v>6</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="str">
         <f>IF(B14="","",SUBTOTAL(3,$B$2:B14))</f>
-        <v>7</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="str">
         <f>IF(B15="","",SUBTOTAL(3,$B$2:B15))</f>
-        <v>8</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="str">
         <f>IF(B16="","",SUBTOTAL(3,$B$2:B16))</f>
-        <v>9</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="str">
         <f>IF(B17="","",SUBTOTAL(3,$B$2:B17))</f>
-        <v>10</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="str">
         <f>IF(B18="","",SUBTOTAL(3,$B$2:B18))</f>
-        <v>11</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="str">
         <f>IF(B19="","",SUBTOTAL(3,$B$2:B19))</f>
-        <v>12</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="str">
         <f>IF(B20="","",SUBTOTAL(3,$B$2:B20))</f>
-        <v>13</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="str">
         <f>IF(B21="","",SUBTOTAL(3,$B$2:B21))</f>
-        <v>14</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="str">
         <f>IF(B22="","",SUBTOTAL(3,$B$2:B22))</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26">
+    <row r="23" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="str">
         <f>IF(B23="","",SUBTOTAL(3,$B$2:B23))</f>
-        <v>15</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>44</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -2169,125 +2069,63 @@
         <f>IF(B24="","",SUBTOTAL(3,$B$2:B24))</f>
         <v/>
       </c>
-      <c r="B24" s="18"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="str">
+    </row>
+    <row r="25" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
         <f>IF(B25="","",SUBTOTAL(3,$B$2:B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="18"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="str">
         <f>IF(B26="","",SUBTOTAL(3,$B$2:B26))</f>
         <v/>
       </c>
-      <c r="B26" s="18"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="str">
         <f>IF(B27="","",SUBTOTAL(3,$B$2:B27))</f>
         <v/>
       </c>
-      <c r="B27" s="18"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="str">
         <f>IF(B28="","",SUBTOTAL(3,$B$2:B28))</f>
         <v/>
       </c>
-      <c r="B28" s="18"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="str">
         <f>IF(B29="","",SUBTOTAL(3,$B$2:B29))</f>
         <v/>
       </c>
-      <c r="B29" s="18"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="str">
         <f>IF(B30="","",SUBTOTAL(3,$B$2:B30))</f>
         <v/>
       </c>
-      <c r="B30" s="18"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="str">
         <f>IF(B31="","",SUBTOTAL(3,$B$2:B31))</f>
         <v/>
       </c>
-      <c r="B31" s="18"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="str">
-        <f>IF(B32="","",SUBTOTAL(3,$B$2:B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="18"/>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="str">
-        <f>IF(B33="","",SUBTOTAL(3,$B$2:B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="18"/>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="str">
-        <f>IF(B34="","",SUBTOTAL(3,$B$2:B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="18"/>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="str">
-        <f>IF(B35="","",SUBTOTAL(3,$B$2:B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="18"/>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="str">
-        <f>IF(B36="","",SUBTOTAL(3,$B$2:B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="18"/>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="str">
-        <f>IF(B37="","",SUBTOTAL(3,$B$2:B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="18"/>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="str">
-        <f>IF(B38="","",SUBTOTAL(3,$B$2:B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="18"/>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="str">
-        <f>IF(B39="","",SUBTOTAL(3,$B$2:B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="18"/>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="str">
-        <f>IF(B40="","",SUBTOTAL(3,$B$2:B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F40">
-    <filterColumn colId="5">
+  <autoFilter ref="A1:F24">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Khẩn cấp - Quan trọng"/>
+        <filter val="Đang làm"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2297,135 +2135,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
-        <f>IF(B2="","",SUBTOTAL(3,$B$2:B2))</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="29">
-        <v>1</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
-        <f>IF(B3="","",SUBTOTAL(3,$B$2:B3))</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
-        <f>IF(B4="","",SUBTOTAL(3,$B$2:B4))</f>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
-        <f>IF(B5="","",SUBTOTAL(3,$B$2:B5))</f>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
-        <f>IF(B6="","",SUBTOTAL(3,$B$2:B6))</f>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="str">
-        <f>IF(B7="","",SUBTOTAL(3,$B$2:B7))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="str">
-        <f>IF(B8="","",SUBTOTAL(3,$B$2:B8))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="str">
-        <f>IF(B9="","",SUBTOTAL(3,$B$2:B9))</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,188 +2162,205 @@
         <v>2</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <f>IF(B2="","",SUBTOTAL(3,$B$2:B2))</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>58</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>51</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D2" s="29">
         <v>1</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <f>IF(B3="","",SUBTOTAL(3,$B$2:B3))</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>52</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="27"/>
       <c r="F3" s="35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <f>IF(B4="","",SUBTOTAL(3,$B$2:B4))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="27"/>
       <c r="F4" s="35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <f>IF(B5="","",SUBTOTAL(3,$B$2:B5))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
       <c r="F5" s="35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <f>IF(B6="","",SUBTOTAL(3,$B$2:B6))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <f>IF(B7="","",SUBTOTAL(3,$B$2:B7))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>92</v>
+        <v>67</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="str">
+      <c r="A8" s="26">
         <f>IF(B8="","",SUBTOTAL(3,$B$2:B8))</f>
-        <v/>
-      </c>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="str">
         <f>IF(B9="","",SUBTOTAL(3,$B$2:B9))</f>
         <v/>
       </c>
+      <c r="B9" s="1"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="str">
         <f>IF(B10="","",SUBTOTAL(3,$B$2:B10))</f>
         <v/>
       </c>
+      <c r="B10" s="18"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="str">
         <f>IF(B11="","",SUBTOTAL(3,$B$2:B11))</f>
         <v/>
       </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="1"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="str">
         <f>IF(B12="","",SUBTOTAL(3,$B$2:B12))</f>
         <v/>
       </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="str">
         <f>IF(B13="","",SUBTOTAL(3,$B$2:B13))</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="str">
         <f>IF(B14="","",SUBTOTAL(3,$B$2:B14))</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="str">
         <f>IF(B15="","",SUBTOTAL(3,$B$2:B15))</f>
         <v/>
       </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="str">
-        <f>IF(B16="","",SUBTOTAL(3,$B$2:B16))</f>
-        <v/>
-      </c>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="A1:F15">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Đang làm"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2650,19 +2381,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="29"/>
@@ -2680,9 +2411,12 @@
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="26">
         <f>IF(B3="","",SUBTOTAL(3,$B$2:B3))</f>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2690,115 +2424,148 @@
         <f>IF(B4="","",SUBTOTAL(3,$B$2:B4))</f>
         <v/>
       </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="str">
         <f>IF(B5="","",SUBTOTAL(3,$B$2:B5))</f>
         <v/>
       </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="str">
         <f>IF(B6="","",SUBTOTAL(3,$B$2:B6))</f>
         <v/>
       </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="str">
         <f>IF(B7="","",SUBTOTAL(3,$B$2:B7))</f>
         <v/>
       </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="str">
         <f>IF(B8="","",SUBTOTAL(3,$B$2:B8))</f>
         <v/>
       </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="str">
         <f>IF(B9="","",SUBTOTAL(3,$B$2:B9))</f>
         <v/>
       </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="str">
         <f>IF(B10="","",SUBTOTAL(3,$B$2:B10))</f>
         <v/>
       </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="str">
         <f>IF(B11="","",SUBTOTAL(3,$B$2:B11))</f>
         <v/>
       </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="str">
         <f>IF(B12="","",SUBTOTAL(3,$B$2:B12))</f>
         <v/>
       </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="str">
         <f>IF(B13="","",SUBTOTAL(3,$B$2:B13))</f>
         <v/>
       </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="str">
         <f>IF(B14="","",SUBTOTAL(3,$B$2:B14))</f>
         <v/>
       </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="str">
         <f>IF(B15="","",SUBTOTAL(3,$B$2:B15))</f>
         <v/>
       </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="str">
         <f>IF(B16="","",SUBTOTAL(3,$B$2:B16))</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="str">
         <f>IF(B17="","",SUBTOTAL(3,$B$2:B17))</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="str">
         <f>IF(B18="","",SUBTOTAL(3,$B$2:B18))</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="str">
         <f>IF(B19="","",SUBTOTAL(3,$B$2:B19))</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="str">
         <f>IF(B20="","",SUBTOTAL(3,$B$2:B20))</f>
         <v/>
       </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2816,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2825,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2837,10 +2604,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2849,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2861,10 +2628,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2872,11 +2639,11 @@
         <f>IF(B6="","",SUBTOTAL(3,$B$2:B6))</f>
         <v>2</v>
       </c>
-      <c r="B6" s="41" t="s">
-        <v>91</v>
+      <c r="B6" s="40" t="s">
+        <v>66</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>